<commit_message>
Changes with ,all assertions working SourceSystemIdentifier	calculationEventTriggers	chargeType	AgreementType	freetime	rateTime	currency	agreementEffectiveDateTime	agreementExpirationDateTime
</commit_message>
<xml_diff>
--- a/src/main/resources/PriceExecutionDataV2- V1.0.xlsx
+++ b/src/main/resources/PriceExecutionDataV2- V1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarshitAgrawal\Documents\v2AutomationTest\kronos-price-execution-v2-suite\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE7C91A-F2F4-4C5D-A0AE-A268798EA91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E355A986-B16F-468C-AB5A-F5EE1B1AEA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D0B60A0E-0E56-41A2-A1DE-4E15E034A992}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="189">
   <si>
     <t>Scenerio</t>
   </si>
@@ -482,13 +482,139 @@
   </si>
   <si>
     <t>TC8</t>
+  </si>
+  <si>
+    <t>INLT4-DET-41868-CONTRACT</t>
+  </si>
+  <si>
+    <t>1-3:17140.0,4-9999:19483.0</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>2024-08-31 23:59:59</t>
+  </si>
+  <si>
+    <t>BDCGP-DET-26015</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1-9999:55.0</t>
+  </si>
+  <si>
+    <t>2024-01-17 00:00:00</t>
+  </si>
+  <si>
+    <t>2049-12-31 23:59:59</t>
+  </si>
+  <si>
+    <t>INLT4-DET-41202</t>
+  </si>
+  <si>
+    <t>1-4:5183.0,5-8:7399.0,9-11:8570.0,12-9999:9741.0</t>
+  </si>
+  <si>
+    <t>2024-02-12 00:00:00</t>
+  </si>
+  <si>
+    <t>INLT4-DET-41549-CONTRACT</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1-4:7399.0,5-7:8570.0,8-9999:9741.0</t>
+  </si>
+  <si>
+    <t>2024-02-06 00:00:00</t>
+  </si>
+  <si>
+    <t>BDCGP-DET-27946-CONTRACT</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1-2:45.0,3-9999:75.0</t>
+  </si>
+  <si>
+    <t>2024-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>BDCGP-DET-26217-STANDARD</t>
+  </si>
+  <si>
+    <t>STANDARD</t>
+  </si>
+  <si>
+    <t>1-3:30.0,4-6:60.0,7-9999:120.0</t>
+  </si>
+  <si>
+    <t>INVTZ-DMR-04593-STANDARD</t>
+  </si>
+  <si>
+    <t>DMR</t>
+  </si>
+  <si>
+    <t>1-12:240.0,13-27:480.0,28-9999:960.0</t>
+  </si>
+  <si>
+    <t>2024-02-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-30 23:59:59</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Dummy scenerios 9</t>
+  </si>
+  <si>
+    <t>dummtt scenerio 9</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>2024-03-27T00:00:00.0+00:00</t>
+  </si>
+  <si>
+    <t>INENN</t>
+  </si>
+  <si>
+    <t>INENNTM</t>
+  </si>
+  <si>
+    <t>003703</t>
+  </si>
+  <si>
+    <t>298604521</t>
+  </si>
+  <si>
+    <t>DB06</t>
+  </si>
+  <si>
+    <t>INENN-DMR-00269-STANDARD</t>
+  </si>
+  <si>
+    <t>1-12:462.3,13-27-923.45,28-9999:1846.9</t>
+  </si>
+  <si>
+    <t>1-9999:120.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +676,15 @@
     <font>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -648,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -735,6 +870,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1061,11 +1214,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A21FA0B-5869-49EF-A56D-6CF6914E02FE}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AX10"/>
+  <dimension ref="A1:AX11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS3" sqref="AS3"/>
+      <selection pane="bottomLeft" activeCell="AQ12" sqref="AQ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.7265625" defaultRowHeight="21"/>
@@ -1096,10 +1249,10 @@
     <col min="35" max="35" width="44.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="49.81640625" style="2" customWidth="1"/>
     <col min="37" max="37" width="34" style="10" customWidth="1"/>
-    <col min="38" max="38" width="34" style="30" customWidth="1"/>
+    <col min="38" max="38" width="56.54296875" style="39" customWidth="1"/>
     <col min="39" max="41" width="33.26953125" style="2" customWidth="1"/>
     <col min="42" max="42" width="21.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.453125" style="2" customWidth="1"/>
+    <col min="43" max="43" width="58.7265625" style="2" customWidth="1"/>
     <col min="44" max="44" width="34.7265625" style="2"/>
     <col min="45" max="45" width="27.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="29.36328125" style="2" bestFit="1" customWidth="1"/>
@@ -1136,44 +1289,44 @@
       <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="35" t="s">
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="34" t="s">
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35" t="s">
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
       <c r="V1" s="17" t="s">
         <v>11</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
       <c r="AH1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1186,7 +1339,7 @@
       <c r="AK1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AL1" s="32" t="s">
+      <c r="AL1" s="36" t="s">
         <v>131</v>
       </c>
       <c r="AM1" s="6" t="s">
@@ -1303,7 +1456,7 @@
         <v>127</v>
       </c>
       <c r="AK2" s="10"/>
-      <c r="AL2" s="21"/>
+      <c r="AL2" s="37"/>
       <c r="AM2" s="6"/>
       <c r="AN2" s="6"/>
       <c r="AO2" s="6"/>
@@ -1424,7 +1577,7 @@
       <c r="AJ3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AL3" s="33" t="s">
+      <c r="AL3" s="38" t="s">
         <v>137</v>
       </c>
       <c r="AM3" s="2" t="s">
@@ -1440,7 +1593,7 @@
         <v>140</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="AR3" s="2" t="s">
         <v>142</v>
@@ -1559,6 +1712,33 @@
       <c r="AJ4" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="AL4" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP4" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="AQ4" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS4" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT4" s="15" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="5" spans="1:50">
       <c r="A5" s="2" t="s">
@@ -1667,6 +1847,33 @@
       <c r="AJ5" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="AL5" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP5" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="AQ5" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT5" s="15" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="6" spans="1:50">
       <c r="A6" s="2" t="s">
@@ -1775,6 +1982,33 @@
       <c r="AJ6" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="AL6" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO6" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP6" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS6" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AT6" s="15" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="7" spans="1:50">
       <c r="A7" s="2" t="s">
@@ -1883,6 +2117,33 @@
       <c r="AJ7" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="AL7" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP7" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="AQ7" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="AR7" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS7" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="AT7" s="15" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8" spans="1:50">
       <c r="A8" s="2" t="s">
@@ -1991,6 +2252,33 @@
       <c r="AJ8" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="AL8" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP8" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="AT8" s="15" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="9" spans="1:50">
       <c r="A9" s="2" t="s">
@@ -2099,10 +2387,37 @@
       <c r="AJ9" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="AL9" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="AM9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO9" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="AQ9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AS9" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT9" s="15" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="10" spans="1:50" ht="21.5" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>146</v>
@@ -2206,10 +2521,167 @@
       <c r="AJ10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
-      <c r="AT10" s="3"/>
+      <c r="AL10" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN10" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP10" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="AQ10" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS10" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="AT10" s="35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50">
+      <c r="A11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="V11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="W11" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="X11" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB11" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL11" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AP11" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AR11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS11" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="AT11" s="15" t="s">
+        <v>155</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="I1:I3" xr:uid="{9A21FA0B-5869-49EF-A56D-6CF6914E02FE}"/>
@@ -2311,44 +2783,44 @@
       <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="35" t="s">
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="34" t="s">
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35" t="s">
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
       <c r="V1" s="17" t="s">
         <v>11</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
       <c r="AH1" s="4" t="s">
         <v>14</v>
       </c>
@@ -3414,6 +3886,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020EE6F886875F3479A7320C651C4BB0A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c572b335d5efd90c651d9a4bfb782d19">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="094134b0-3d77-4420-9192-38b55bfdb847" xmlns:ns4="87e327b4-1c67-4c79-9504-651b5c762153" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ba886b1631b68cf8d3bd78a7376db11" ns3:_="" ns4:_="">
     <xsd:import namespace="094134b0-3d77-4420-9192-38b55bfdb847"/>
@@ -3596,22 +4083,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1988DBA0-35D5-4CC5-AE8C-DAD94579179D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0885CBCF-8660-4136-917D-CFB4CC058676}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C83059C-CF3F-405E-87A1-D64449759DDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3628,21 +4117,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0885CBCF-8660-4136-917D-CFB4CC058676}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1988DBA0-35D5-4CC5-AE8C-DAD94579179D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Seprate into more methods for more redabiliy
</commit_message>
<xml_diff>
--- a/src/main/resources/PriceExecutionDataV2- V1.0.xlsx
+++ b/src/main/resources/PriceExecutionDataV2- V1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarshitAgrawal\Documents\v2AutomationTest\kronos-price-execution-v2-suite\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarshitAgrawal\Documents\v2 from git\kronos-price-execution-v2-suite\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E355A986-B16F-468C-AB5A-F5EE1B1AEA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6164BA89-0BE5-4D0E-8109-C08E2B833DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D0B60A0E-0E56-41A2-A1DE-4E15E034A992}"/>
   </bookViews>
@@ -3886,21 +3886,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020EE6F886875F3479A7320C651C4BB0A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c572b335d5efd90c651d9a4bfb782d19">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="094134b0-3d77-4420-9192-38b55bfdb847" xmlns:ns4="87e327b4-1c67-4c79-9504-651b5c762153" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ba886b1631b68cf8d3bd78a7376db11" ns3:_="" ns4:_="">
     <xsd:import namespace="094134b0-3d77-4420-9192-38b55bfdb847"/>
@@ -4083,24 +4068,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1988DBA0-35D5-4CC5-AE8C-DAD94579179D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0885CBCF-8660-4136-917D-CFB4CC058676}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C83059C-CF3F-405E-87A1-D64449759DDA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4117,4 +4100,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0885CBCF-8660-4136-917D-CFB4CC058676}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1988DBA0-35D5-4CC5-AE8C-DAD94579179D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>